<commit_message>
Further work on Blik
</commit_message>
<xml_diff>
--- a/MirrorMe/Statements.xlsx
+++ b/MirrorMe/Statements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="615" windowWidth="19815" windowHeight="7305" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="615" windowWidth="19815" windowHeight="7305" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Statements" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>Statement</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
 </sst>
 </file>
@@ -433,7 +445,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A10"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +471,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,6 +483,9 @@
       <c r="B1" t="s">
         <v>9</v>
       </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -479,6 +494,9 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -487,6 +505,9 @@
       <c r="B3" t="s">
         <v>16</v>
       </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -495,6 +516,9 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -502,6 +526,9 @@
       </c>
       <c r="B5" t="s">
         <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -565,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -628,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>